<commit_message>
test: Set correct numConditions and update tests
</commit_message>
<xml_diff>
--- a/matlab_code/tests/ensembleFxns/testFiles/toy_model1_freeExchange.xlsx
+++ b/matlab_code/tests/ensembleFxns/testFiles/toy_model1_freeExchange.xlsx
@@ -483,7 +483,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -537,7 +537,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,7 +612,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="B3 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -758,7 +758,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B3 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -981,7 +981,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B3 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1302,7 +1302,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L2" activeCellId="1" sqref="B3 L2"/>
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1612,7 +1612,7 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B3 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2549,7 +2549,7 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="1" sqref="B3 I13"/>
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2871,7 +2871,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="1" sqref="B3 D1"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3056,7 +3056,7 @@
   <dimension ref="A2:A15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B3 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3153,7 +3153,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B3 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3285,7 +3285,7 @@
   <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="B3 A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3417,7 +3417,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B3 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3598,7 +3598,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="1" sqref="B3 H13"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>